<commit_message>
New test data files added
</commit_message>
<xml_diff>
--- a/Test_Data/appium_data.xlsx
+++ b/Test_Data/appium_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/animeshmukherjee/Desktop/Personal/Animesh/tripledot_assignment/Test_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829C4082-36D4-6641-8AE0-9BD90C6281B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C400B69-A7C2-8E4A-B0E2-29B78356724A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="3080" windowWidth="21600" windowHeight="11360" activeTab="1" xr2:uid="{E4A251DD-F0BA-B24E-BB12-1E97DEE930FB}"/>
+    <workbookView xWindow="3080" yWindow="3080" windowWidth="21600" windowHeight="11360" xr2:uid="{E4A251DD-F0BA-B24E-BB12-1E97DEE930FB}"/>
   </bookViews>
   <sheets>
     <sheet name="happy_path_data" sheetId="2" r:id="rId1"/>
@@ -26,15 +26,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>test123@email.com</t>
+    <t>animesh5678@gmail.com</t>
   </si>
   <si>
-    <t>sheree@email.com</t>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Welcome@1</t>
+  </si>
+  <si>
+    <t>validuser2233@email.com</t>
   </si>
 </sst>
 </file>
@@ -99,10 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18EA071-6A31-024D-939A-0E99E4FDC5F9}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,7 +442,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -446,10 +453,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8305F6A-4031-D142-9847-A91A53A5A3F8}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,14 +464,20 @@
     <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>